<commit_message>
cleaned data to some extent, little more is left
</commit_message>
<xml_diff>
--- a/mathTransformed/HMPSTT_(2015-07-01)_47_3.xlsx
+++ b/mathTransformed/HMPSTT_(2015-07-01)_47_3.xlsx
@@ -1817,7 +1817,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Bangalore -5</t>
+          <t>Bengaluru (Bangalore) Rural</t>
         </is>
       </c>
     </row>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Sevaashram High School Srirampuram Bangalore -2</t>
+          <t>Bengaluru (Bangalore) Urban</t>
         </is>
       </c>
     </row>

</xml_diff>